<commit_message>
Małe poprawki i dodatki
Took 1 hour 55 minutes
</commit_message>
<xml_diff>
--- a/src/main/resources/kryteria_oceny_GUI_webowe_Java_2020 (1).xlsx
+++ b/src/main/resources/kryteria_oceny_GUI_webowe_Java_2020 (1).xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_7EF6A0EE21A1C7FA2B2F7B1FED194F4FA25A30D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\razoh\Desktop\Kantor1\Kantor\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5AD6EC-4C1C-4AEC-9D3D-BC88C1316F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27960" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -17,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Kryteria oceny technicznej projektu związanego z tworzeniem GUI w jezyku Java</t>
   </si>
@@ -232,6 +235,48 @@
   </si>
   <si>
     <t>Ocena końcowa (średnia arytmetyczna):</t>
+  </si>
+  <si>
+    <t>klienci</t>
+  </si>
+  <si>
+    <t>waluta</t>
+  </si>
+  <si>
+    <t>wartość waluty</t>
+  </si>
+  <si>
+    <t>adres</t>
+  </si>
+  <si>
+    <t>nowa tranakcja</t>
+  </si>
+  <si>
+    <t>dodawanie pracownika</t>
+  </si>
+  <si>
+    <t>edycja pracownika</t>
+  </si>
+  <si>
+    <t>Exchange Rate</t>
+  </si>
+  <si>
+    <t>wszystkie</t>
+  </si>
+  <si>
+    <t>złożone</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -293,12 +338,18 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -354,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -384,6 +435,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,9 +495,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -472,7 +535,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -578,7 +641,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -752,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -768,27 +831,30 @@
     <col min="6" max="6" width="14.25" customWidth="1"/>
     <col min="7" max="7" width="18.375" customWidth="1"/>
     <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="18">
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:13">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:13">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:13" ht="15">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -796,7 +862,7 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -806,7 +872,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="18">
+    <row r="8" spans="1:13" ht="18">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -832,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -855,8 +921,23 @@
         <v>6</v>
       </c>
       <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="30">
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -879,8 +960,17 @@
         <v>6</v>
       </c>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="15">
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="36.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -904,7 +994,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -923,12 +1013,12 @@
       <c r="F12" s="3">
         <v>7</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="15">
         <v>8</v>
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:13" ht="51.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -938,7 +1028,7 @@
       <c r="C13" s="3">
         <v>2</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="15">
         <v>3</v>
       </c>
       <c r="E13" s="3">
@@ -952,7 +1042,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="71.25">
+    <row r="14" spans="1:13" ht="71.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -976,7 +1066,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="28.5">
+    <row r="15" spans="1:13" ht="28.5">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1090,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="42.75">
+    <row r="16" spans="1:13" ht="42.75">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1037,7 +1127,7 @@
       <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1062,10 +1152,10 @@
         <v>45</v>
       </c>
       <c r="E18" s="12"/>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
@@ -1135,7 +1225,7 @@
       <c r="F21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="16" t="s">
         <v>59</v>
       </c>
       <c r="H21" s="6"/>
@@ -1175,6 +1265,71 @@
         <v>67</v>
       </c>
       <c r="H24" s="6"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <f>SUM(B29:F29)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>SUM(B30:F30)</f>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1183,7 +1338,7 @@
     <mergeCell ref="A6:H6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1344,6 +1499,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1352,20 +1513,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4D3BC4-54BE-40B7-A801-6573AEF5D70A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4D3BC4-54BE-40B7-A801-6573AEF5D70A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bcab37e4-82f5-46fe-bc9e-fd348a7ee16a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950AD74-1941-4DBE-A075-340795A34881}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FFFF51-DB15-4D8C-AB03-217253165B29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FFFF51-DB15-4D8C-AB03-217253165B29}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950AD74-1941-4DBE-A075-340795A34881}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Validation + Exceptions Handlers
Took 2 hours 35 minutes
</commit_message>
<xml_diff>
--- a/src/main/resources/kryteria_oceny_GUI_webowe_Java_2020 (1).xlsx
+++ b/src/main/resources/kryteria_oceny_GUI_webowe_Java_2020 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\razoh\Desktop\Kantor1\Kantor\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5AD6EC-4C1C-4AEC-9D3D-BC88C1316F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DAD85F-96DD-4135-AF9E-75715D1CD9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t>Kryteria oceny technicznej projektu związanego z tworzeniem GUI w jezyku Java</t>
   </si>
@@ -277,6 +277,18 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>podgląda kursów walut</t>
+  </si>
+  <si>
+    <t>podgląd klientów</t>
+  </si>
+  <si>
+    <t>pogdląd klienta, jego adresów oraz histori wymian</t>
+  </si>
+  <si>
+    <t>histroia tranksakcji</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -425,10 +437,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -437,17 +461,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -833,6 +848,7 @@
     <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -863,14 +879,14 @@
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="8" spans="1:13" ht="18">
       <c r="A8" s="2" t="s">
@@ -914,26 +930,26 @@
       <c r="E9" s="3">
         <v>4</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
         <v>5</v>
       </c>
       <c r="G9" s="3">
         <v>6</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" t="s">
+      <c r="I9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="19" t="s">
         <v>72</v>
       </c>
     </row>
@@ -947,7 +963,7 @@
       <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="11">
         <v>3</v>
       </c>
       <c r="E10" s="3">
@@ -960,15 +976,17 @@
         <v>6</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" t="s">
+      <c r="I10" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="19" t="s">
         <v>68</v>
       </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="36.75" customHeight="1">
       <c r="A11" s="3" t="s">
@@ -983,7 +1001,7 @@
       <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="11">
         <v>4</v>
       </c>
       <c r="F11" s="3">
@@ -993,6 +1011,19 @@
         <v>6</v>
       </c>
       <c r="H11" s="4"/>
+      <c r="I11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" ht="30">
       <c r="A12" s="3" t="s">
@@ -1013,7 +1044,7 @@
       <c r="F12" s="3">
         <v>7</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="11">
         <v>8</v>
       </c>
       <c r="H12" s="4"/>
@@ -1028,7 +1059,7 @@
       <c r="C13" s="3">
         <v>2</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>3</v>
       </c>
       <c r="E13" s="3">
@@ -1127,7 +1158,7 @@
       <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="12" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1148,14 +1179,14 @@
       <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="14"/>
+      <c r="F18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="18"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
@@ -1225,7 +1256,7 @@
       <c r="F21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="12" t="s">
         <v>59</v>
       </c>
       <c r="H21" s="6"/>
@@ -1367,6 +1398,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010056B0C48163DE9F45B643DD78596E34ED" ma:contentTypeVersion="2" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="3b641c6d60780d1d51c12dd77a82bf19">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcab37e4-82f5-46fe-bc9e-fd348a7ee16a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8cc1b275399b6305173f3ac5d5cf88f" ns2:_="">
     <xsd:import namespace="bcab37e4-82f5-46fe-bc9e-fd348a7ee16a"/>
@@ -1498,12 +1535,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1514,6 +1545,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FFFF51-DB15-4D8C-AB03-217253165B29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4D3BC4-54BE-40B7-A801-6573AEF5D70A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1531,15 +1571,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FFFF51-DB15-4D8C-AB03-217253165B29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950AD74-1941-4DBE-A075-340795A34881}">
   <ds:schemaRefs>

</xml_diff>